<commit_message>
Changed to use shell command to unzip
</commit_message>
<xml_diff>
--- a/public/ZxTemplate.xlsx
+++ b/public/ZxTemplate.xlsx
@@ -23,7 +23,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>#{address}</t>
+    <t>Shinagawa</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -34,7 +34,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>#{name}</t>
+    <t>Chubachi</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>

</xml_diff>

<commit_message>
Rewrited the replace function
</commit_message>
<xml_diff>
--- a/public/ZxTemplate.xlsx
+++ b/public/ZxTemplate.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>住所</t>
     <rPh sb="0" eb="2">
@@ -35,6 +35,14 @@
   </si>
   <si>
     <t>Chubachi</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>140</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>〒</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -440,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -462,6 +470,14 @@
       </c>
       <c r="B2" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>